<commit_message>
leave func for employee
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -60,7 +60,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,19 +450,74 @@
           <t>TÊN</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>04/06/2023</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>05/06/2023</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>06/06/2023</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>08/06/2023</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>09/06/2023</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>10/06/2023</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>11/06/2023</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>12/06/2023</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>13/06/2023</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>14/06/2023</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>15/06/2023</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>16/06/2023</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>17/06/2023</t>
         </is>
       </c>
     </row>
@@ -474,14 +529,77 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Nguyễn  Hoàng Khởi</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr"/>
-      <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>x/2</t>
+          <t>Nguyễn Hoàng Khởi</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>X/2</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>X/2</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="M2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="N2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="O2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
         </is>
       </c>
     </row>
@@ -496,11 +614,156 @@
           <t>Lê Trung Hậu</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr"/>
-      <c r="D3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="P3" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>190501013</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Lê Yến Nhi</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="O4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="P4" s="3" t="inlineStr">
+        <is>
+          <t>KP</t>
         </is>
       </c>
     </row>

</xml_diff>